<commit_message>
supratim531: (Modified the old schema as per new plan of backend) Update the .xlsx
</commit_message>
<xml_diff>
--- a/database/book.xlsx
+++ b/database/book.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUPRATIM\Desktop\IEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUPRATIM\Desktop\BookShoppingApp\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>A</t>
   </si>
@@ -121,9 +121,6 @@
     <t>9/C, Belgachia Road</t>
   </si>
   <si>
-    <t>CUSTOMER_ADDRESS</t>
-  </si>
-  <si>
     <t>BOOK</t>
   </si>
   <si>
@@ -217,7 +214,10 @@
     <t>ORDERS</t>
   </si>
   <si>
-    <t>ORDERS_BOOK</t>
+    <t>ORDER_DETAILS</t>
+  </si>
+  <si>
+    <t>DETAILS_ID</t>
   </si>
 </sst>
 </file>
@@ -285,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -299,6 +299,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -616,16 +622,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
@@ -694,7 +702,7 @@
         <v>7003378772</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -714,7 +722,7 @@
         <v>7003378773</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -741,7 +749,9 @@
       <c r="F8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -762,6 +772,9 @@
       <c r="F9" s="4">
         <v>700020</v>
       </c>
+      <c r="G9" s="3">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -782,6 +795,9 @@
       <c r="F10" s="4">
         <v>600078</v>
       </c>
+      <c r="G10" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -802,6 +818,9 @@
       <c r="F11" s="4">
         <v>700037</v>
       </c>
+      <c r="G11" s="4">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -810,528 +829,497 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>16</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1200</v>
+      </c>
+      <c r="D15" s="4">
+        <v>120</v>
+      </c>
+      <c r="E15" s="4">
+        <v>850</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="4">
+        <v>800</v>
+      </c>
+      <c r="D16" s="4">
+        <v>75</v>
+      </c>
+      <c r="E16" s="4">
+        <v>670</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1300</v>
+      </c>
+      <c r="D17" s="4">
+        <v>195</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="4">
+        <v>90</v>
+      </c>
+      <c r="E18" s="4">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="4">
+        <v>950</v>
+      </c>
+      <c r="D19" s="4">
+        <v>50</v>
+      </c>
+      <c r="E19" s="4">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1200</v>
-      </c>
-      <c r="D21" s="4">
-        <v>120</v>
-      </c>
-      <c r="E21" s="4">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>22</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="4">
-        <v>800</v>
-      </c>
-      <c r="D22" s="4">
-        <v>75</v>
-      </c>
-      <c r="E22" s="4">
-        <v>670</v>
+      <c r="B22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1300</v>
-      </c>
-      <c r="D23" s="4">
-        <v>195</v>
-      </c>
-      <c r="E23" s="4">
-        <v>1250</v>
+        <v>46</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D24" s="4">
-        <v>90</v>
-      </c>
-      <c r="E24" s="4">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>25</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="4">
-        <v>950</v>
-      </c>
-      <c r="D25" s="4">
-        <v>50</v>
-      </c>
-      <c r="E25" s="4">
-        <v>990</v>
+        <v>48</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>46</v>
+      <c r="A28" s="4">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4">
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
+        <v>22</v>
+      </c>
+      <c r="B29" s="4">
         <v>31</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
+        <v>23</v>
+      </c>
+      <c r="B30" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>24</v>
+      </c>
+      <c r="B31" s="4">
         <v>32</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="4">
+        <v>25</v>
+      </c>
+      <c r="B32" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>25</v>
+      </c>
+      <c r="B33" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>21</v>
-      </c>
-      <c r="B34" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>22</v>
-      </c>
-      <c r="B35" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>23</v>
-      </c>
-      <c r="B36" s="4">
-        <v>31</v>
+      <c r="B36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B37" s="4">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B38" s="4">
-        <v>31</v>
+        <v>42</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
+        <v>53</v>
+      </c>
+      <c r="B39" s="4">
+        <v>41</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>54</v>
+      </c>
+      <c r="B40" s="4">
+        <v>43</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>55</v>
+      </c>
+      <c r="B41" s="4">
+        <v>41</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>56</v>
+      </c>
+      <c r="B42" s="4">
+        <v>42</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>71</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4">
+        <v>51</v>
+      </c>
+      <c r="D46" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>72</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="4">
+        <v>52</v>
+      </c>
+      <c r="D47" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>73</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4">
+        <v>52</v>
+      </c>
+      <c r="D48" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>74</v>
+      </c>
+      <c r="B49" s="4">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4">
+        <v>53</v>
+      </c>
+      <c r="D49" s="4">
         <v>25</v>
       </c>
-      <c r="B39" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F42" s="6" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>75</v>
+      </c>
+      <c r="B50" s="4">
+        <v>3</v>
+      </c>
+      <c r="C50" s="4">
         <v>54</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="D50" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>76</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1</v>
+      </c>
+      <c r="C51" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>51</v>
-      </c>
-      <c r="B43" s="4">
-        <v>12</v>
-      </c>
-      <c r="C43" s="4">
-        <v>42</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="D51" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>77</v>
+      </c>
+      <c r="B52" s="4">
+        <v>2</v>
+      </c>
+      <c r="C52" s="4">
         <v>56</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>52</v>
-      </c>
-      <c r="B44" s="4">
-        <v>12</v>
-      </c>
-      <c r="C44" s="4">
-        <v>42</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="D52" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>78</v>
+      </c>
+      <c r="B53" s="4">
+        <v>3</v>
+      </c>
+      <c r="C53" s="4">
         <v>56</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>53</v>
-      </c>
-      <c r="B45" s="4">
-        <v>11</v>
-      </c>
-      <c r="C45" s="4">
-        <v>41</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>54</v>
-      </c>
-      <c r="B46" s="4">
-        <v>13</v>
-      </c>
-      <c r="C46" s="4">
-        <v>43</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>55</v>
-      </c>
-      <c r="B47" s="4">
-        <v>11</v>
-      </c>
-      <c r="C47" s="4">
-        <v>41</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>56</v>
-      </c>
-      <c r="B48" s="4">
-        <v>12</v>
-      </c>
-      <c r="C48" s="4">
-        <v>42</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>61</v>
-      </c>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>51</v>
-      </c>
-      <c r="B52" s="4">
-        <v>21</v>
-      </c>
-      <c r="C52" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>52</v>
-      </c>
-      <c r="B53" s="4">
-        <v>22</v>
-      </c>
-      <c r="C53" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>52</v>
-      </c>
-      <c r="B54" s="4">
+      <c r="D53" s="4">
         <v>23</v>
       </c>
-      <c r="C54" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
-        <v>53</v>
-      </c>
-      <c r="B55" s="4">
-        <v>25</v>
-      </c>
-      <c r="C55" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
-        <v>54</v>
-      </c>
-      <c r="B56" s="4">
-        <v>24</v>
-      </c>
-      <c r="C56" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
-        <v>55</v>
-      </c>
-      <c r="B57" s="4">
-        <v>21</v>
-      </c>
-      <c r="C57" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
-        <v>56</v>
-      </c>
-      <c r="B58" s="4">
-        <v>21</v>
-      </c>
-      <c r="C58" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
-        <v>56</v>
-      </c>
-      <c r="B59" s="4">
-        <v>23</v>
-      </c>
-      <c r="C59" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="1"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
     <hyperlink ref="F4" r:id="rId2"/>
     <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="C29" r:id="rId4"/>
-    <hyperlink ref="C30" r:id="rId5"/>
+    <hyperlink ref="C23" r:id="rId4"/>
+    <hyperlink ref="C24" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>